<commit_message>
linky_data_t + contract + tarif
</commit_message>
<xml_diff>
--- a/firmware/tramesLinky/datas.xlsx
+++ b/firmware/tramesLinky/datas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\08-LocalRepos\TICMeter\firmware\tramesLinky\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232BA369-1E25-4A2B-B682-0D68637F7C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3587F9B-FE61-49AE-A47C-1DE9B28ABBDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{DF9CA697-8C6D-478C-8E2E-59A27A25127B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="250">
   <si>
     <t>label 1 (Hist)</t>
   </si>
@@ -784,6 +784,9 @@
   </si>
   <si>
     <t>SMAXSN-1</t>
+  </si>
+  <si>
+    <t>N° jours en cours fournisseur</t>
   </si>
 </sst>
 </file>
@@ -885,8 +888,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -896,14 +899,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -950,7 +946,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D27E242-3ECB-4B3A-AA2C-237703A5A098}" name="Tableau1" displayName="Tableau1" ref="A1:M90" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4D27E242-3ECB-4B3A-AA2C-237703A5A098}" name="Tableau1" displayName="Tableau1" ref="A1:M90" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:M90" xr:uid="{4D27E242-3ECB-4B3A-AA2C-237703A5A098}"/>
   <tableColumns count="13">
     <tableColumn id="6" xr3:uid="{7BF275E3-5B88-462C-99C2-AE692F3D047B}" name="NOM"/>
@@ -1272,7 +1268,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G7" sqref="G7"/>
+      <selection pane="topRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,7 +1289,7 @@
     <col min="16" max="16" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="11" customFormat="1" ht="66.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="11" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>209</v>
       </c>
@@ -3408,7 +3404,7 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>124</v>
+        <v>249</v>
       </c>
       <c r="D84" t="s">
         <v>210</v>

</xml_diff>